<commit_message>
Updated more files in server
</commit_message>
<xml_diff>
--- a/templates/metrologia/ejemplo-sensores.xlsx
+++ b/templates/metrologia/ejemplo-sensores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DANI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DANI\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81694494-AB51-4973-89B6-A6B5E3019C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F61DFBD-EDE6-4F9A-82A9-68686B843653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{92F233CF-B524-4A54-B391-7545C32DAF25}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{92F233CF-B524-4A54-B391-7545C32DAF25}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="53">
   <si>
     <t>Emitido el</t>
   </si>
@@ -183,6 +183,18 @@
   </si>
   <si>
     <t>Certificado Name</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Secundario</t>
+  </si>
+  <si>
+    <t>Vencido</t>
+  </si>
+  <si>
+    <t>Primario</t>
   </si>
 </sst>
 </file>
@@ -535,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5BD41EE-E4B4-4C08-B398-78B7E6346E27}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +558,7 @@
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -568,8 +580,11 @@
       <c r="G1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -591,8 +606,11 @@
       <c r="G2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -614,8 +632,11 @@
       <c r="G3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -637,8 +658,11 @@
       <c r="G4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -660,8 +684,11 @@
       <c r="G5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -683,8 +710,11 @@
       <c r="G6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -706,8 +736,11 @@
       <c r="G7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -729,8 +762,11 @@
       <c r="G8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -752,8 +788,11 @@
       <c r="G9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -775,8 +814,11 @@
       <c r="G10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -798,8 +840,11 @@
       <c r="G11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -821,8 +866,11 @@
       <c r="G12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -844,8 +892,11 @@
       <c r="G13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -867,8 +918,11 @@
       <c r="G14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -890,8 +944,11 @@
       <c r="G15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -913,8 +970,11 @@
       <c r="G16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -936,8 +996,11 @@
       <c r="G17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -959,8 +1022,11 @@
       <c r="G18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -982,8 +1048,11 @@
       <c r="G19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1005,8 +1074,11 @@
       <c r="G20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1028,8 +1100,11 @@
       <c r="G21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1050,6 +1125,9 @@
       </c>
       <c r="G22" t="s">
         <v>31</v>
+      </c>
+      <c r="H22" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>